<commit_message>
Desenho Conceitual, Logico, Fisico do banco
</commit_message>
<xml_diff>
--- a/01-QuadroBranco/Exemplo de Telas.xlsx
+++ b/01-QuadroBranco/Exemplo de Telas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f5fd9d0a02b8421/IBMR/2020.2/06 - Laboratório de Sofware e Projetos/00-Projeto/01-QuadroBranco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="8_{71691130-73D3-4981-8353-2D4D97D248EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{01084484-119C-4253-90EE-E5EB7EC9ABBB}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{71691130-73D3-4981-8353-2D4D97D248EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5B256F8C-9F11-473A-A216-A86D46FE0421}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-255" windowWidth="29040" windowHeight="15840" xr2:uid="{56A3317A-48B3-4AB8-B6CA-95F3D6C13AB7}"/>
+    <workbookView xWindow="32220" yWindow="2145" windowWidth="21600" windowHeight="13425" xr2:uid="{56A3317A-48B3-4AB8-B6CA-95F3D6C13AB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="56">
   <si>
     <t>Turno Manhã A</t>
   </si>
@@ -141,12 +141,75 @@
   </si>
   <si>
     <t>Fim</t>
+  </si>
+  <si>
+    <t>Sab/Dom</t>
+  </si>
+  <si>
+    <t>Sab</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Hora Extra</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>Pagaamento</t>
+  </si>
+  <si>
+    <t>Gestor</t>
+  </si>
+  <si>
+    <t>Funcionario</t>
+  </si>
+  <si>
+    <t>Aprovacao</t>
+  </si>
+  <si>
+    <t>joao</t>
+  </si>
+  <si>
+    <t>APROVAÇÃO DE HORAS</t>
+  </si>
+  <si>
+    <t>BANCO DE HORAS</t>
+  </si>
+  <si>
+    <t>Onde guardar o valor maximo de horas</t>
+  </si>
+  <si>
+    <t>onde gardar o calor das horas de banco</t>
+  </si>
+  <si>
+    <t>HoraExtra</t>
+  </si>
+  <si>
+    <t>HoraFeriado</t>
+  </si>
+  <si>
+    <t>jornada</t>
+  </si>
+  <si>
+    <t>Entrada</t>
+  </si>
+  <si>
+    <t>Saida</t>
+  </si>
+  <si>
+    <t>Almoço</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -287,11 +350,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -325,6 +425,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,15 +758,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C13289-9997-4ADA-AAC3-1B6B3701013E}">
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10:T13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
     <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18.28515625" customWidth="1"/>
@@ -1213,32 +1335,429 @@
       <c r="W29" s="23"/>
     </row>
     <row r="30" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="I30" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" t="s">
+        <v>19</v>
+      </c>
       <c r="T30" s="22"/>
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
       <c r="W30" s="23"/>
     </row>
     <row r="31" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="H31" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>8</v>
+      </c>
       <c r="T31" s="22"/>
       <c r="U31" s="10"/>
       <c r="V31" s="10"/>
       <c r="W31" s="23"/>
     </row>
     <row r="32" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="H32" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>9</v>
+      </c>
       <c r="T32" s="22"/>
       <c r="U32" s="10"/>
       <c r="V32" s="10"/>
       <c r="W32" s="23"/>
     </row>
-    <row r="33" spans="20:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" t="s">
+        <v>10</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33" t="s">
+        <v>10</v>
+      </c>
       <c r="T33" s="24"/>
       <c r="U33" s="25"/>
       <c r="V33" s="25"/>
       <c r="W33" s="26"/>
     </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="H34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34">
+        <v>4</v>
+      </c>
+      <c r="L34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>5</v>
+      </c>
+      <c r="L35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="K36">
+        <v>6</v>
+      </c>
+      <c r="L36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="K37">
+        <v>7</v>
+      </c>
+      <c r="L37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>8</v>
+      </c>
+      <c r="L38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" t="s">
+        <v>54</v>
+      </c>
+      <c r="F39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C40" s="41">
+        <v>0</v>
+      </c>
+      <c r="D40" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E40" s="41">
+        <f>C40+SUM(D40,F40)</f>
+        <v>0.375</v>
+      </c>
+      <c r="F40" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="41">
+        <f>E40</f>
+        <v>0.375</v>
+      </c>
+      <c r="D41" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E41" s="41">
+        <f t="shared" ref="E41:E44" si="0">C41+SUM(D41,F41)</f>
+        <v>0.75</v>
+      </c>
+      <c r="F41" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="T41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="41">
+        <f>E41</f>
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E42" s="41">
+        <f t="shared" si="0"/>
+        <v>1.125</v>
+      </c>
+      <c r="F42" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="40"/>
+    </row>
+    <row r="43" spans="3:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D43" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E43" s="41">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="F43" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="4"/>
+      <c r="P43" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q43" s="35"/>
+    </row>
+    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C44" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D44" s="41">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E44" s="41">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="F44" s="1">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="I44" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L44" s="6"/>
+      <c r="P44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q44" s="36">
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="45" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+      <c r="H45" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="31">
+        <v>44079</v>
+      </c>
+      <c r="J45" s="32">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K45" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L45" s="6"/>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45" t="s">
+        <v>40</v>
+      </c>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="6"/>
+    </row>
+    <row r="46" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="G46" s="5"/>
+      <c r="H46" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="31">
+        <v>44080</v>
+      </c>
+      <c r="J46" s="32">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K46" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L46" s="6"/>
+      <c r="M46">
+        <v>2</v>
+      </c>
+      <c r="N46" t="s">
+        <v>50</v>
+      </c>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="6"/>
+    </row>
+    <row r="47" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="G47" s="5"/>
+      <c r="H47" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="31">
+        <v>44081</v>
+      </c>
+      <c r="J47" s="32">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K47" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="L47" s="37"/>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="N47" t="s">
+        <v>51</v>
+      </c>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="6"/>
+    </row>
+    <row r="48" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="G48" s="5"/>
+      <c r="H48" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="31">
+        <v>44082</v>
+      </c>
+      <c r="J48" s="32">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K48" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L48" s="6"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="6"/>
+    </row>
+    <row r="49" spans="7:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G49" s="5"/>
+      <c r="H49" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="31">
+        <v>44083</v>
+      </c>
+      <c r="J49" s="32">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K49" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L49" s="6"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="9"/>
+    </row>
+    <row r="50" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G50" s="5"/>
+      <c r="H50" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I50" s="31">
+        <v>44083</v>
+      </c>
+      <c r="J50" s="32">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="K50" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L50" s="6"/>
+    </row>
+    <row r="51" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G51" s="5"/>
+      <c r="H51" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I51" s="31">
+        <v>44083</v>
+      </c>
+      <c r="J51" s="32">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="K51" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="L51" s="6"/>
+    </row>
+    <row r="52" spans="7:17" x14ac:dyDescent="0.25">
+      <c r="G52" s="5"/>
+      <c r="H52" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I52" s="31">
+        <v>44083</v>
+      </c>
+      <c r="J52" s="32">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="K52" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="L52" s="6"/>
+    </row>
+    <row r="53" spans="7:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G53" s="7"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G42:L42"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K45:K52" xr:uid="{7862DAC2-AD4F-4602-8136-E625805794BC}">
+      <formula1>$M$45:$M$46</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>